<commit_message>
started on contract PDF. This is initial layout using html2pdf canvas
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Email Contract</t>
   </si>
@@ -66,6 +66,36 @@
   </si>
   <si>
     <t>Remove Payment Method CC on Contract Page before contract</t>
+  </si>
+  <si>
+    <t>Submit Transaction Data to BOSS</t>
+  </si>
+  <si>
+    <t>Create asptheade transaction number</t>
+  </si>
+  <si>
+    <t>enter asptitemd and aspttendd after</t>
+  </si>
+  <si>
+    <t>Enter Token into strcustr</t>
+  </si>
+  <si>
+    <t>Save CC last 4 digits and cvv exp date</t>
+  </si>
+  <si>
+    <t>Create ONLINE Boss account</t>
+  </si>
+  <si>
+    <t>Script to OPEN / CLOSE Drawer</t>
+  </si>
+  <si>
+    <t>Ifee for Online? JoAnna? Add a For Web column in ifee table?</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>CLEANUP</t>
   </si>
 </sst>
 </file>
@@ -101,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,82 +414,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B14"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>13</v>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45778</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding legal guardian to contractpage and enforcing requirement
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Email Contract</t>
   </si>
@@ -96,6 +96,93 @@
   </si>
   <si>
     <t>CLEANUP</t>
+  </si>
+  <si>
+    <t>Tax Rate from BOSS and apply to pages</t>
+  </si>
+  <si>
+    <t>Prorate $0 ? How do we implement this?</t>
+  </si>
+  <si>
+    <t>Add Legal Guardian Info to Contract and PDF</t>
+  </si>
+  <si>
+    <t>Nanny requires enter the Nanny info as a Dependent to the Account with their Info</t>
+  </si>
+  <si>
+    <t>Unlimited Child Care in NM applies directly to the number of Children added to the membership, so 3 kids = 1,2,3 Unlimited as options &amp; Only applies to 11 and under kids</t>
+  </si>
+  <si>
+    <t>Adding multiple youths and children need to be put back</t>
+  </si>
+  <si>
+    <t>Nanny only applies if Child/Youth have been added to Membership</t>
+  </si>
+  <si>
+    <t>Nanny turns membership into Family in New Mexico or Dual in Colorado</t>
+  </si>
+  <si>
+    <t>Confirm if 14 Day Term starts on Signature Date or Start Date</t>
+  </si>
+  <si>
+    <t>SYP in Colorado can have Couple SYP or Individual with multiple children</t>
+  </si>
+  <si>
+    <t>SYP in New Mexico is Individual Only</t>
+  </si>
+  <si>
+    <t>Changing Membership Type isn't always clearing?</t>
+  </si>
+  <si>
+    <t>181818 Junior has different options</t>
+  </si>
+  <si>
+    <t>CONTRACT</t>
+  </si>
+  <si>
+    <t>CC PROCESSING</t>
+  </si>
+  <si>
+    <t>CONVERGE</t>
+  </si>
+  <si>
+    <t>FLUIDPAY</t>
+  </si>
+  <si>
+    <t>ONLINE DRAWER</t>
+  </si>
+  <si>
+    <t>NANNY</t>
+  </si>
+  <si>
+    <t>SYP</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>JUNIOR</t>
+  </si>
+  <si>
+    <t>UNLIMITED CHILD CARE</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t>TABLES</t>
+  </si>
+  <si>
+    <t>INSERT asprecdoc</t>
+  </si>
+  <si>
+    <t>Move all data from Web tables to Production</t>
   </si>
 </sst>
 </file>
@@ -111,12 +198,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,9 +224,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,123 +509,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45778</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1">
-        <v>45778</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>21</v>
+      <c r="B61" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Legal guardian to contract and pdf contract
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Email Contract</t>
   </si>
@@ -183,14 +183,31 @@
   </si>
   <si>
     <t>Move all data from Web tables to Production</t>
+  </si>
+  <si>
+    <t>Start Date can not be greater than 7 days from signup.</t>
+  </si>
+  <si>
+    <t>Start Date per John P</t>
+  </si>
+  <si>
+    <t>Add Descriptive popups for Addons - what they are</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -224,11 +241,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,17 +529,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -531,7 +551,7 @@
       <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -556,7 +576,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -577,7 +597,7 @@
       <c r="B10" s="3">
         <v>45797</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
@@ -589,12 +609,19 @@
       <c r="I11" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -651,7 +678,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -666,7 +693,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -677,7 +704,7 @@
       <c r="B31" s="3">
         <v>45778</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
@@ -688,7 +715,7 @@
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -708,7 +735,7 @@
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -718,7 +745,7 @@
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="C42" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -733,7 +760,7 @@
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+      <c r="C46" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -742,81 +769,109 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="3">
         <v>45797</v>
       </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="6"/>
       <c r="D54" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B61" s="3">
         <v>45797</v>
       </c>
-      <c r="C61" s="2"/>
+      <c r="C61" s="6"/>
       <c r="D61" s="2" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D63" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding demo pay and then goes to confirmation
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>Email Contract</t>
   </si>
@@ -532,7 +532,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,14 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45805</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="1"/>

</xml_diff>

<commit_message>
making minor changes per JoAnna, added /mo, Junior title, etc.
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Email Contract</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Add Descriptive popups for Addons - what they are</t>
+  </si>
+  <si>
+    <t>INSERT ALL WEB TABLES</t>
   </si>
 </sst>
 </file>
@@ -215,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +228,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -241,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -249,6 +258,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,330 +562,354 @@
       <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="C2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45805</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>0</v>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>2</v>
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3">
-        <v>45797</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
+      <c r="D10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3">
-        <v>45805</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="1"/>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
-        <v>38</v>
+      <c r="E13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3">
-        <v>45798</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="2" t="s">
-        <v>4</v>
+      <c r="D14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>18</v>
+      <c r="B20" s="1"/>
+      <c r="C20" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="E22" t="s">
-        <v>15</v>
+      <c r="D22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
-        <v>50</v>
+      <c r="D23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>51</v>
+      <c r="C26" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
-        <v>41</v>
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45778</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="C31" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="3">
-        <v>45778</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>45811</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3">
+        <v>45811</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="5" t="s">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="5" t="s">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54" s="3">
-        <v>45797</v>
-      </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="3">
-        <v>45798</v>
-      </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G59" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="3">
-        <v>45797</v>
-      </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" s="3">
-        <v>45798</v>
-      </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D63" s="4" t="s">
-        <v>55</v>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data persistence to save data via browser local storage
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Email Contract</t>
   </si>
@@ -195,6 +195,27 @@
   </si>
   <si>
     <t>INSERT ALL WEB TABLES</t>
+  </si>
+  <si>
+    <t>Insert Membership information into Web tables</t>
+  </si>
+  <si>
+    <t>After the CC is processed, perform a qry of the cust_code to make sure it is still available</t>
+  </si>
+  <si>
+    <t>if not available get new one and update web table</t>
+  </si>
+  <si>
+    <t>if available continue</t>
+  </si>
+  <si>
+    <t>Insert Membership information into Production tables</t>
+  </si>
+  <si>
+    <t>Insert Transaction into Transaction tables with this cust_code</t>
+  </si>
+  <si>
+    <t>So, half the data is being stored in web and transaction tables go straight to production</t>
   </si>
 </sst>
 </file>
@@ -542,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,48 +677,73 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="E17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="E18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -709,17 +755,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Got data submitting to web tables strcustr, asamembr, asacontr,asprecdoc,asamessag
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>Email Contract</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>So, half the data is being stored in web and transaction tables go straight to production</t>
+  </si>
+  <si>
+    <t>Taxes in asprecdoc? Seems mixed on existing - ask John/Mel</t>
+  </si>
+  <si>
+    <t>offer PIN/Password to customer</t>
   </si>
 </sst>
 </file>
@@ -561,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,112 +732,105 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
       <c r="G24" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G25" t="s">
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B28" s="3">
         <v>45778</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="2" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="8" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B33" s="3">
         <v>45811</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="2" t="s">
+      <c r="C33" s="6"/>
+      <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="5" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B38" s="3">
         <v>45797</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="2" t="s">
+      <c r="C38" s="6"/>
+      <c r="D38" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="3">
-        <v>45798</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -839,11 +838,14 @@
         <v>22</v>
       </c>
       <c r="B42" s="3">
-        <v>45811</v>
+        <v>45798</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="G42" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,11 +853,11 @@
         <v>22</v>
       </c>
       <c r="B43" s="3">
-        <v>45797</v>
+        <v>45811</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -863,98 +865,110 @@
         <v>22</v>
       </c>
       <c r="B44" s="3">
-        <v>45798</v>
+        <v>45797</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="4" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="4"/>
-    </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="7" t="s">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="7" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="7" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="7" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="5" t="s">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated enrollment confirmation layout
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18855" windowHeight="7275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>Email Contract</t>
   </si>
@@ -570,7 +570,7 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,30 +668,64 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="D16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="E17" t="s">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="E18" t="s">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -708,7 +742,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G21" t="s">
@@ -716,7 +757,14 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H22" t="s">
@@ -724,7 +772,14 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H23" t="s">
@@ -732,7 +787,14 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G24" t="s">
@@ -770,7 +832,14 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+      <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -824,7 +893,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+      <c r="A40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added fluidpay processor page and matched converge processor page
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t>Email Contract</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>offer PIN/Password to customer</t>
+  </si>
+  <si>
+    <t>Colorado contract</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,19 +605,12 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3">
-        <v>45797</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -622,61 +618,61 @@
         <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>45805</v>
+        <v>45797</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45805</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3">
         <v>45798</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="2" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3">
-        <v>45868</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -688,7 +684,7 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -700,7 +696,7 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -711,9 +707,8 @@
         <v>45868</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
-        <v>15</v>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,34 +721,32 @@
       <c r="C18" s="6"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3">
-        <v>45868</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -765,10 +758,10 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -778,12 +771,12 @@
       <c r="B23" s="3">
         <v>45868</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,42 +786,45 @@
       <c r="B24" s="3">
         <v>45868</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3">
-        <v>45778</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -836,92 +832,89 @@
         <v>22</v>
       </c>
       <c r="B29" s="3">
-        <v>45868</v>
+        <v>45778</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="8" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3">
         <v>45811</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="2" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="3">
         <v>45797</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="2" t="s">
+      <c r="C39" s="6"/>
+      <c r="D39" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="3">
         <v>45868</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="2" t="s">
+      <c r="C41" s="6"/>
+      <c r="D41" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="3">
-        <v>45798</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,11 +922,14 @@
         <v>22</v>
       </c>
       <c r="B43" s="3">
-        <v>45811</v>
+        <v>45798</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="G43" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -941,11 +937,11 @@
         <v>22</v>
       </c>
       <c r="B44" s="3">
-        <v>45797</v>
+        <v>45811</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -953,98 +949,110 @@
         <v>22</v>
       </c>
       <c r="B45" s="3">
-        <v>45798</v>
+        <v>45797</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="4" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="4"/>
-    </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="7" t="s">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="7" t="s">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="7" t="s">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="7" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="7" t="s">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="5" t="s">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made the colorado/denver canvascontract.pdf
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Email Contract</t>
   </si>
@@ -573,7 +573,7 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +599,14 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
emails are correct and contracts are being created properly
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Email Contract</t>
   </si>
@@ -225,13 +225,19 @@
   </si>
   <si>
     <t>Colorado contract</t>
+  </si>
+  <si>
+    <t>Move CC authorize to CC Payment Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this correct in emails? Includes monthly dues, add-ons, and applicable taxes </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +252,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -280,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -290,6 +302,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +627,14 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45875</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -645,65 +668,58 @@
       </c>
       <c r="I7" s="1"/>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3">
         <v>45798</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="2" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="3">
-        <v>45868</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3">
-        <v>45868</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -715,7 +731,7 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,9 +742,8 @@
         <v>45868</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>15</v>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -739,51 +754,46 @@
         <v>45868</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3">
-        <v>45868</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3">
-        <v>45868</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,12 +803,12 @@
       <c r="B24" s="3">
         <v>45868</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H24" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -810,101 +820,114 @@
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45868</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G27" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="3">
         <v>45778</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="2" t="s">
+      <c r="C31" s="6"/>
+      <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3">
         <v>45868</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="2" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="8" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="3">
         <v>45811</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="2" t="s">
+      <c r="C36" s="6"/>
+      <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="3">
-        <v>45797</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -912,16 +935,16 @@
         <v>22</v>
       </c>
       <c r="B41" s="3">
-        <v>45868</v>
+        <v>45797</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,26 +952,16 @@
         <v>22</v>
       </c>
       <c r="B43" s="3">
-        <v>45798</v>
+        <v>45868</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="3">
-        <v>45811</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="2" t="s">
-        <v>35</v>
+      <c r="D44" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,11 +969,14 @@
         <v>22</v>
       </c>
       <c r="B45" s="3">
-        <v>45797</v>
+        <v>45798</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="G45" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,98 +984,122 @@
         <v>22</v>
       </c>
       <c r="B46" s="3">
-        <v>45798</v>
+        <v>45811</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3">
+        <v>45797</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="3">
+        <v>45798</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="4" t="s">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="7" t="s">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="7" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="7" t="s">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="7" t="s">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="5" t="s">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created direct club links
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>Email Contract</t>
   </si>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -304,6 +304,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -589,7 +592,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +681,14 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="10" t="s">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45879</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="11" t="s">
         <v>68</v>
       </c>
     </row>
@@ -713,7 +723,15 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45879</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1015,65 +1033,72 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3">
+        <v>45879</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C51" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C56" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C59" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
still working in pretend environment for executive meeting 8-21 corrected more things for colorado
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>Email Contract</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t xml:space="preserve">Is this correct in emails? Includes monthly dues, add-ons, and applicable taxes </t>
+  </si>
+  <si>
+    <t>Need to add Ifee to items being sent to database, need to get the upc code</t>
+  </si>
+  <si>
+    <t>Kids names need to be upper case</t>
+  </si>
+  <si>
+    <t>Remove just Dues from colorado contract and show total only</t>
   </si>
 </sst>
 </file>
@@ -589,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,82 +1058,109 @@
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="5" t="s">
-        <v>23</v>
+      <c r="C66" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
for company wide testing using pretend payment
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>Email Contract</t>
   </si>
@@ -240,6 +240,13 @@
   </si>
   <si>
     <t>Remove just Dues from colorado contract and show total only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add (applicable taxes not included)
+</t>
+  </si>
+  <si>
+    <t>Both contracts need to say Enrollment Fee and show the value</t>
   </si>
 </sst>
 </file>
@@ -301,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -317,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,10 +691,14 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="4" t="s">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45889</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2" t="s">
         <v>67</v>
       </c>
       <c r="I8" s="1"/>
@@ -732,15 +746,11 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="3">
-        <v>45879</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1042,7 +1052,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>22</v>
       </c>
@@ -1054,62 +1064,73 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D51" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="4" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="3">
+        <v>45889</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
fixed dtored draft data so it properly restores again and removed unused payment files
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>Email Contract</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Both contracts need to say Enrollment Fee and show the value</t>
+  </si>
+  <si>
+    <t>Need to add Ifee to transactions</t>
+  </si>
+  <si>
+    <t>Add dropdown for Sales Reps to main page</t>
   </si>
 </sst>
 </file>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,88 +1106,101 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D57" s="4"/>
+      <c r="D57" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C58" s="7" t="s">
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C61" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C63" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="5" t="s">
-        <v>23</v>
+      <c r="C73" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>12</v>
+      <c r="C76" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added enrollment fee to both contracts
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -249,10 +249,10 @@
     <t>Both contracts need to say Enrollment Fee and show the value</t>
   </si>
   <si>
-    <t>Need to add Ifee to transactions</t>
-  </si>
-  <si>
     <t>Add dropdown for Sales Reps to main page</t>
+  </si>
+  <si>
+    <t>Add Club logos to contracts</t>
   </si>
 </sst>
 </file>
@@ -614,9 +614,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -1074,35 +1074,35 @@
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="4" t="s">
-        <v>69</v>
+      <c r="A51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="3">
+        <v>45889</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="3">
-        <v>45889</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D53" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="E54" s="12" t="s">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E53" s="12" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D55" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1122,85 +1122,82 @@
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D60" s="4"/>
+      <c r="C60" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="7" t="s">
-        <v>42</v>
+      <c r="D61" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
+      <c r="D66" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="7" t="s">
-        <v>43</v>
+      <c r="D69" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
+      <c r="D73" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="5" t="s">
-        <v>23</v>
+      <c r="D76" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added code for fluidpay customer vault. not fully functional yet
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>Email Contract</t>
   </si>
@@ -331,7 +331,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -617,7 +617,7 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,17 +1086,40 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="4" t="s">
+      <c r="A52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="3">
+        <v>45909</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="3">
+        <v>45909</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="2"/>
       <c r="E53" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D54" s="4" t="s">
+      <c r="A54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="3">
+        <v>45909</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="2" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected tax to show 3 digits pass decimal, corrected start date to allow today
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
   <si>
     <t>Email Contract</t>
   </si>
@@ -253,13 +254,91 @@
   </si>
   <si>
     <t>Add Club logos to contracts</t>
+  </si>
+  <si>
+    <t>Add logs for who is using the site and decline cc transactions</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Change Taxes to show 3 digits</t>
+  </si>
+  <si>
+    <t>Add Enrollment to Transaction</t>
+  </si>
+  <si>
+    <t>Change Requested Start Date to Include Today and up to 29 Days</t>
+  </si>
+  <si>
+    <t>Converge CC Processing</t>
+  </si>
+  <si>
+    <t>Fluidpay CC Processing</t>
+  </si>
+  <si>
+    <t>Highpoint Junior Rate</t>
+  </si>
+  <si>
+    <t>Highpoint Remove Racquet Addons</t>
+  </si>
+  <si>
+    <t>Monaco Remove Tennis Passport and Racquet Addons</t>
+  </si>
+  <si>
+    <t>Offer to Create PIN/Password to Customer</t>
+  </si>
+  <si>
+    <t>Download App text in Confirmation</t>
+  </si>
+  <si>
+    <t>Add Logos to Contracts</t>
+  </si>
+  <si>
+    <t>Save PDF Contracts to Membership Accounting</t>
+  </si>
+  <si>
+    <t>Create Logs of Visitors</t>
+  </si>
+  <si>
+    <t>Move to Production Server</t>
+  </si>
+  <si>
+    <t>Link Wellbridge.com to App (John Love)</t>
+  </si>
+  <si>
+    <t>Cleanup</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Contract - base on actual membership type</t>
+  </si>
+  <si>
+    <t>Unlimited Childcare</t>
+  </si>
+  <si>
+    <t>Nanny</t>
+  </si>
+  <si>
+    <t>Multiple Junior Options</t>
+  </si>
+  <si>
+    <t>SYP Additional Rules</t>
+  </si>
+  <si>
+    <t>Add a way to Enter Enrollment Fees</t>
+  </si>
+  <si>
+    <t>Add a way to Enter Prorate Fees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +359,15 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -314,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -334,6 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1218,14 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D56" s="4" t="s">
+      <c r="A56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="3">
+        <v>45912</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1139,7 +1235,9 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D59" s="4"/>
@@ -1205,7 +1303,7 @@
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
+      <c r="D76" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1228,4 +1326,155 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Converge CC Processing that is working - need to capture token and cc info to database still
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
   <si>
     <t>Email Contract</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>Add a way to Enter Prorate Fees</t>
+  </si>
+  <si>
+    <t>per JoAnna and John keep it at 7 days</t>
+  </si>
+  <si>
+    <t>removed from inventory per John</t>
   </si>
 </sst>
 </file>
@@ -1330,147 +1336,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3">
+        <v>45922</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>45922</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>45922</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>45922</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added sales reps and their emp code
</commit_message>
<xml_diff>
--- a/Online Enrollment Check Listxlsx.xlsx
+++ b/Online Enrollment Check Listxlsx.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>Email Contract</t>
   </si>
@@ -337,7 +337,7 @@
     <t>per JoAnna and John keep it at 7 days</t>
   </si>
   <si>
-    <t>removed from inventory per John</t>
+    <t>removed from inventory per John - I removed from web_addons</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1385,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="A4" s="3">
+        <v>45923</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1406,9 +1412,11 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>45922</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>45923</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>85</v>
       </c>

</xml_diff>